<commit_message>
Commit before merging gayatri-models
</commit_message>
<xml_diff>
--- a/docs/04_data_design/schema (v2.3).xlsx
+++ b/docs/04_data_design/schema (v2.3).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Farheen\OBE-TRACKING-SYSTEM\docs\04_data_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF4A7EC-A002-415C-BBEB-BC50BD777FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913350F9-2D42-4037-AB24-635D86F51157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="766">
   <si>
     <t>name</t>
   </si>
@@ -2339,12 +2339,256 @@
   <si>
     <t>m5: survey_submission_guard</t>
   </si>
+  <si>
+    <t>user_id (fk)</t>
+  </si>
+  <si>
+    <t>no need remove</t>
+  </si>
+  <si>
+    <t>add updated at</t>
+  </si>
+  <si>
+    <t>types are diff, look assessments/models.py/class assessment</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Here, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>weightage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is just </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>internal distribution inside ONE course</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>unique_together = (</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>'course_id'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>'assessment_name'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>'academic_year'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>'semester'</t>
+    </r>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>Meta:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    unique_together = (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>'assessment_id'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>'co_id'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    unique_together = (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>'assessment_id'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>'student_id'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>remove constraint</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2391,6 +2635,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFCF8E6D"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2406,7 +2673,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2466,11 +2733,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2503,12 +2781,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2526,6 +2798,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2809,11 +3096,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O436"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="71" zoomScaleNormal="71" zoomScaleSheetLayoutView="35" workbookViewId="0">
-      <selection activeCell="J138" sqref="J138"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="71" zoomScaleNormal="71" zoomScaleSheetLayoutView="35" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -2824,26 +3111,26 @@
     <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:15" ht="18">
+      <c r="A1" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.6">
+      <c r="A3" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -2860,7 +3147,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="34.200000000000003" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>155</v>
       </c>
@@ -2877,7 +3164,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="34.200000000000003" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2894,7 +3181,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="43.2">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2912,7 +3199,7 @@
       </c>
       <c r="O7" s="13"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -2930,7 +3217,7 @@
       </c>
       <c r="O8" s="13"/>
     </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="28.8">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2947,7 +3234,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="24" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -2964,7 +3251,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="39" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -2981,7 +3268,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="47.4" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -2998,7 +3285,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13" s="2" t="s">
         <v>501</v>
       </c>
@@ -3015,16 +3302,16 @@
         <v>505</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:15" ht="15.6">
+      <c r="A15" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-    </row>
-    <row r="16" spans="1:15" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="1:15" ht="24.6" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -3041,7 +3328,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="24.6" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -3058,7 +3345,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="26.4" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -3075,7 +3362,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="41.4" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>506</v>
       </c>
@@ -3092,18 +3379,18 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
+    <row r="20" spans="1:6" ht="25.8" customHeight="1"/>
+    <row r="21" spans="1:6" ht="15.6">
+      <c r="A21" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-    </row>
-    <row r="22" spans="1:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6" ht="34.200000000000003" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -3123,7 +3410,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="43.2">
       <c r="A23" s="2" t="s">
         <v>156</v>
       </c>
@@ -3143,7 +3430,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -3161,7 +3448,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="28.8">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -3179,7 +3466,7 @@
       </c>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="28.8">
       <c r="A26" s="2" t="s">
         <v>418</v>
       </c>
@@ -3197,7 +3484,7 @@
       </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="22.8" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3215,7 +3502,7 @@
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="26.4" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -3233,7 +3520,7 @@
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="28.2" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
@@ -3251,7 +3538,7 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="34.200000000000003" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -3269,7 +3556,7 @@
       </c>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="33.6" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
@@ -3287,7 +3574,7 @@
       </c>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="43.2" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -3305,7 +3592,7 @@
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="37.200000000000003" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>16</v>
       </c>
@@ -3323,7 +3610,7 @@
       </c>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="37.200000000000003" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>501</v>
       </c>
@@ -3341,17 +3628,17 @@
       </c>
       <c r="F34" s="2"/>
     </row>
-    <row r="36" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="20" t="s">
+    <row r="36" spans="1:6" ht="15.6">
+      <c r="A36" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
@@ -3371,7 +3658,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="72">
       <c r="A38" s="2" t="s">
         <v>157</v>
       </c>
@@ -3391,7 +3678,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="28.8">
       <c r="A39" s="2" t="s">
         <v>82</v>
       </c>
@@ -3409,7 +3696,7 @@
       </c>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="28.8">
       <c r="A40" s="2" t="s">
         <v>86</v>
       </c>
@@ -3427,7 +3714,7 @@
       </c>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="28.8">
       <c r="A41" s="2" t="s">
         <v>90</v>
       </c>
@@ -3445,7 +3732,7 @@
       </c>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="28.8">
       <c r="A42" s="2" t="s">
         <v>12</v>
       </c>
@@ -3463,7 +3750,7 @@
       </c>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="43.2">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -3481,7 +3768,7 @@
       </c>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="28.8">
       <c r="A44" s="2" t="s">
         <v>98</v>
       </c>
@@ -3499,7 +3786,7 @@
       </c>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
         <v>501</v>
       </c>
@@ -3517,26 +3804,26 @@
       </c>
       <c r="F45" s="2"/>
     </row>
-    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A48" s="19" t="s">
+    <row r="48" spans="1:6" ht="18">
+      <c r="A48" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-    </row>
-    <row r="50" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="20" t="s">
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+    </row>
+    <row r="50" spans="1:5" ht="15.6">
+      <c r="A50" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -3553,7 +3840,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -3570,7 +3857,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="28.8">
       <c r="A53" s="2" t="s">
         <v>103</v>
       </c>
@@ -3587,7 +3874,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="28.8">
       <c r="A54" s="2" t="s">
         <v>14</v>
       </c>
@@ -3604,7 +3891,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="28.8">
       <c r="A55" s="2" t="s">
         <v>16</v>
       </c>
@@ -3621,7 +3908,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="14.4" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>501</v>
       </c>
@@ -3638,16 +3925,16 @@
         <v>505</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="20" t="s">
+    <row r="58" spans="1:5" ht="15.6">
+      <c r="A58" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
         <v>20</v>
       </c>
@@ -3664,7 +3951,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5">
       <c r="A60" s="2" t="s">
         <v>114</v>
       </c>
@@ -3681,7 +3968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5">
       <c r="A61" s="2" t="s">
         <v>108</v>
       </c>
@@ -3698,7 +3985,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5">
       <c r="A62" s="2" t="s">
         <v>109</v>
       </c>
@@ -3715,7 +4002,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="28.8">
       <c r="A63" s="2" t="s">
         <v>110</v>
       </c>
@@ -3732,7 +4019,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5">
       <c r="A64" s="2" t="s">
         <v>14</v>
       </c>
@@ -3749,7 +4036,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="28.8">
       <c r="A65" s="2" t="s">
         <v>16</v>
       </c>
@@ -3766,7 +4053,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="14.4" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>501</v>
       </c>
@@ -3783,17 +4070,17 @@
         <v>505</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="20" t="s">
+    <row r="68" spans="1:6" ht="15.6">
+      <c r="A68" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="1" t="s">
         <v>20</v>
       </c>
@@ -3813,7 +4100,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" ht="43.2">
       <c r="A70" s="2" t="s">
         <v>86</v>
       </c>
@@ -3833,7 +4120,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="28.8">
       <c r="A71" s="2" t="s">
         <v>112</v>
       </c>
@@ -3851,7 +4138,7 @@
       </c>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6">
       <c r="A72" s="2" t="s">
         <v>113</v>
       </c>
@@ -3869,7 +4156,7 @@
       </c>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6">
       <c r="A73" s="2" t="s">
         <v>12</v>
       </c>
@@ -3887,7 +4174,7 @@
       </c>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="28.8">
       <c r="A74" s="2" t="s">
         <v>8</v>
       </c>
@@ -3905,7 +4192,7 @@
       </c>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="14.4" customHeight="1">
       <c r="A75" s="2" t="s">
         <v>114</v>
       </c>
@@ -3923,7 +4210,7 @@
       </c>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6">
       <c r="A76" s="2" t="s">
         <v>14</v>
       </c>
@@ -3941,7 +4228,7 @@
       </c>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="28.8">
       <c r="A77" s="2" t="s">
         <v>16</v>
       </c>
@@ -3959,7 +4246,7 @@
       </c>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6">
       <c r="A78" s="2" t="s">
         <v>501</v>
       </c>
@@ -3977,17 +4264,17 @@
       </c>
       <c r="F78" s="2"/>
     </row>
-    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="15" t="s">
+    <row r="80" spans="1:6" ht="15.6">
+      <c r="A80" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="1" t="s">
         <v>20</v>
       </c>
@@ -4007,7 +4294,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="43.2">
       <c r="A82" s="2" t="s">
         <v>131</v>
       </c>
@@ -4027,7 +4314,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="14.4" customHeight="1">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -4045,7 +4332,7 @@
       </c>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="28.8">
       <c r="A84" s="2" t="s">
         <v>116</v>
       </c>
@@ -4063,7 +4350,7 @@
       </c>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7">
       <c r="A85" s="2" t="s">
         <v>107</v>
       </c>
@@ -4081,7 +4368,7 @@
       </c>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7">
       <c r="A86" s="2" t="s">
         <v>14</v>
       </c>
@@ -4099,7 +4386,7 @@
       </c>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="28.8">
       <c r="A87" s="2" t="s">
         <v>16</v>
       </c>
@@ -4117,7 +4404,7 @@
       </c>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7">
       <c r="A88" s="2" t="s">
         <v>501</v>
       </c>
@@ -4135,17 +4422,17 @@
       </c>
       <c r="F88" s="2"/>
     </row>
-    <row r="90" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="20" t="s">
+    <row r="90" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A90" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="B90" s="20"/>
-      <c r="C90" s="20"/>
-      <c r="D90" s="20"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="20"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="1" t="s">
         <v>20</v>
       </c>
@@ -4165,7 +4452,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="43.2">
       <c r="A92" s="2" t="s">
         <v>133</v>
       </c>
@@ -4184,8 +4471,11 @@
       <c r="F92" s="2" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G92" s="22" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="28.8">
       <c r="A93" s="2" t="s">
         <v>8</v>
       </c>
@@ -4202,8 +4492,11 @@
         <v>122</v>
       </c>
       <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G93" s="22" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="2" t="s">
         <v>123</v>
       </c>
@@ -4221,7 +4514,7 @@
       </c>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7">
       <c r="A95" s="2" t="s">
         <v>107</v>
       </c>
@@ -4239,7 +4532,7 @@
       </c>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7">
       <c r="A96" s="2" t="s">
         <v>14</v>
       </c>
@@ -4257,7 +4550,7 @@
       </c>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="28.8">
       <c r="A97" s="2" t="s">
         <v>16</v>
       </c>
@@ -4275,7 +4568,7 @@
       </c>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12">
       <c r="A98" s="2" t="s">
         <v>501</v>
       </c>
@@ -4293,18 +4586,18 @@
       </c>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="20" t="s">
+    <row r="99" spans="1:12" ht="14.4" customHeight="1"/>
+    <row r="100" spans="1:12" ht="15.6">
+      <c r="A100" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="B100" s="20"/>
-      <c r="C100" s="20"/>
-      <c r="D100" s="20"/>
-      <c r="E100" s="20"/>
-      <c r="F100" s="20"/>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B100" s="18"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" s="1" t="s">
         <v>20</v>
       </c>
@@ -4324,7 +4617,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" ht="43.2">
       <c r="A102" s="2" t="s">
         <v>138</v>
       </c>
@@ -4344,7 +4637,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" ht="28.8">
       <c r="A103" s="2" t="s">
         <v>8</v>
       </c>
@@ -4362,7 +4655,7 @@
       </c>
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12">
       <c r="A104" s="2" t="s">
         <v>128</v>
       </c>
@@ -4381,7 +4674,7 @@
       <c r="F104" s="2"/>
       <c r="L104" s="8"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12">
       <c r="A105" s="2" t="s">
         <v>107</v>
       </c>
@@ -4399,7 +4692,7 @@
       </c>
       <c r="F105" s="2"/>
     </row>
-    <row r="106" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" ht="14.4" customHeight="1">
       <c r="A106" s="2" t="s">
         <v>14</v>
       </c>
@@ -4417,7 +4710,7 @@
       </c>
       <c r="F106" s="2"/>
     </row>
-    <row r="107" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" ht="28.8">
       <c r="A107" s="2" t="s">
         <v>16</v>
       </c>
@@ -4435,7 +4728,7 @@
       </c>
       <c r="F107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12">
       <c r="A108" s="2" t="s">
         <v>501</v>
       </c>
@@ -4453,17 +4746,17 @@
       </c>
       <c r="F108" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="20" t="s">
+    <row r="110" spans="1:12" ht="15.6">
+      <c r="A110" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="B110" s="20"/>
-      <c r="C110" s="20"/>
-      <c r="D110" s="20"/>
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-    </row>
-    <row r="111" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="18"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+    </row>
+    <row r="111" spans="1:12" ht="12" customHeight="1">
       <c r="A111" s="1" t="s">
         <v>20</v>
       </c>
@@ -4483,7 +4776,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" ht="28.8">
       <c r="A112" s="2" t="s">
         <v>141</v>
       </c>
@@ -4503,7 +4796,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="28.8">
       <c r="A113" s="2" t="s">
         <v>131</v>
       </c>
@@ -4521,7 +4814,7 @@
       </c>
       <c r="F113" s="2"/>
     </row>
-    <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="28.8">
       <c r="A114" s="2" t="s">
         <v>133</v>
       </c>
@@ -4539,7 +4832,7 @@
       </c>
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="28.8">
       <c r="A115" s="2" t="s">
         <v>135</v>
       </c>
@@ -4557,7 +4850,7 @@
       </c>
       <c r="F115" s="2"/>
     </row>
-    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="28.8">
       <c r="A116" s="2" t="s">
         <v>16</v>
       </c>
@@ -4575,7 +4868,7 @@
       </c>
       <c r="F116" s="2"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6">
       <c r="A117" s="2" t="s">
         <v>501</v>
       </c>
@@ -4593,20 +4886,20 @@
       </c>
       <c r="F117" s="2"/>
     </row>
-    <row r="118" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="18">
       <c r="A118" s="7"/>
     </row>
-    <row r="119" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="20" t="s">
+    <row r="119" spans="1:6" ht="15.6">
+      <c r="A119" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="B119" s="21"/>
-      <c r="C119" s="21"/>
-      <c r="D119" s="21"/>
-      <c r="E119" s="21"/>
-      <c r="F119" s="21"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B119" s="19"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" s="1" t="s">
         <v>20</v>
       </c>
@@ -4626,7 +4919,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="28.8">
       <c r="A121" s="2" t="s">
         <v>141</v>
       </c>
@@ -4646,7 +4939,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="28.8">
       <c r="A122" s="2" t="s">
         <v>131</v>
       </c>
@@ -4664,7 +4957,7 @@
       </c>
       <c r="F122" s="2"/>
     </row>
-    <row r="123" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="28.8">
       <c r="A123" s="2" t="s">
         <v>138</v>
       </c>
@@ -4682,7 +4975,7 @@
       </c>
       <c r="F123" s="2"/>
     </row>
-    <row r="124" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="28.8">
       <c r="A124" s="2" t="s">
         <v>135</v>
       </c>
@@ -4700,7 +4993,7 @@
       </c>
       <c r="F124" s="2"/>
     </row>
-    <row r="125" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="28.8">
       <c r="A125" s="2" t="s">
         <v>16</v>
       </c>
@@ -4718,7 +5011,7 @@
       </c>
       <c r="F125" s="2"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6">
       <c r="A126" s="2" t="s">
         <v>501</v>
       </c>
@@ -4736,17 +5029,17 @@
       </c>
       <c r="F126" s="2"/>
     </row>
-    <row r="128" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" s="20" t="s">
+    <row r="128" spans="1:6" ht="15.6">
+      <c r="A128" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="B128" s="20"/>
-      <c r="C128" s="20"/>
-      <c r="D128" s="20"/>
-      <c r="E128" s="20"/>
-      <c r="F128" s="20"/>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B128" s="18"/>
+      <c r="C128" s="18"/>
+      <c r="D128" s="18"/>
+      <c r="E128" s="18"/>
+      <c r="F128" s="18"/>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" s="1" t="s">
         <v>20</v>
       </c>
@@ -4766,7 +5059,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" ht="43.2">
       <c r="A130" s="2" t="s">
         <v>9</v>
       </c>
@@ -4786,7 +5079,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6">
       <c r="A131" s="2" t="s">
         <v>140</v>
       </c>
@@ -4804,7 +5097,7 @@
       </c>
       <c r="F131" s="2"/>
     </row>
-    <row r="132" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" ht="28.8">
       <c r="A132" s="2" t="s">
         <v>8</v>
       </c>
@@ -4822,7 +5115,7 @@
       </c>
       <c r="F132" s="2"/>
     </row>
-    <row r="133" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" ht="28.8">
       <c r="A133" s="2" t="s">
         <v>114</v>
       </c>
@@ -4840,7 +5133,7 @@
       </c>
       <c r="F133" s="2"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6">
       <c r="A134" s="2" t="s">
         <v>14</v>
       </c>
@@ -4858,7 +5151,7 @@
       </c>
       <c r="F134" s="2"/>
     </row>
-    <row r="135" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" ht="28.8">
       <c r="A135" s="2" t="s">
         <v>16</v>
       </c>
@@ -4876,7 +5169,7 @@
       </c>
       <c r="F135" s="2"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6">
       <c r="A136" s="2" t="s">
         <v>501</v>
       </c>
@@ -4894,17 +5187,17 @@
       </c>
       <c r="F136" s="2"/>
     </row>
-    <row r="138" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="15" t="s">
+    <row r="138" spans="1:6" ht="15.6">
+      <c r="A138" s="20" t="s">
         <v>723</v>
       </c>
-      <c r="B138" s="15"/>
-      <c r="C138" s="15"/>
-      <c r="D138" s="15"/>
-      <c r="E138" s="15"/>
-      <c r="F138" s="15"/>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B138" s="20"/>
+      <c r="C138" s="20"/>
+      <c r="D138" s="20"/>
+      <c r="E138" s="20"/>
+      <c r="F138" s="20"/>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" s="1" t="s">
         <v>20</v>
       </c>
@@ -4924,7 +5217,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6">
       <c r="A140" s="2" t="s">
         <v>702</v>
       </c>
@@ -4942,7 +5235,7 @@
       </c>
       <c r="F140" s="2"/>
     </row>
-    <row r="141" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" ht="57.6">
       <c r="A141" s="2" t="s">
         <v>131</v>
       </c>
@@ -4962,7 +5255,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" ht="28.8">
       <c r="A142" s="2" t="s">
         <v>90</v>
       </c>
@@ -4980,7 +5273,7 @@
       </c>
       <c r="F142" s="2"/>
     </row>
-    <row r="143" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" ht="43.2">
       <c r="A143" s="2" t="s">
         <v>9</v>
       </c>
@@ -5000,7 +5293,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" ht="28.8">
       <c r="A144" s="2" t="s">
         <v>713</v>
       </c>
@@ -5020,7 +5313,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" ht="28.8">
       <c r="A145" s="2" t="s">
         <v>717</v>
       </c>
@@ -5038,7 +5331,7 @@
       </c>
       <c r="F145" s="2"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
         <v>14</v>
       </c>
@@ -5056,7 +5349,7 @@
       </c>
       <c r="F146" s="2"/>
     </row>
-    <row r="147" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" ht="28.8">
       <c r="A147" s="2" t="s">
         <v>16</v>
       </c>
@@ -5074,7 +5367,7 @@
       </c>
       <c r="F147" s="2"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6">
       <c r="A148" s="9"/>
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
@@ -5082,27 +5375,27 @@
       <c r="E148" s="9"/>
       <c r="F148" s="9"/>
     </row>
-    <row r="150" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A150" s="19" t="s">
+    <row r="150" spans="1:6" ht="18">
+      <c r="A150" s="17" t="s">
         <v>419</v>
       </c>
-      <c r="B150" s="19"/>
-      <c r="C150" s="19"/>
-      <c r="D150" s="19"/>
-      <c r="E150" s="19"/>
-      <c r="F150" s="19"/>
-    </row>
-    <row r="152" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A152" s="20" t="s">
+      <c r="B150" s="17"/>
+      <c r="C150" s="17"/>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="17"/>
+    </row>
+    <row r="152" spans="1:6" ht="15.6">
+      <c r="A152" s="18" t="s">
         <v>420</v>
       </c>
-      <c r="B152" s="20"/>
-      <c r="C152" s="20"/>
-      <c r="D152" s="20"/>
-      <c r="E152" s="20"/>
+      <c r="B152" s="18"/>
+      <c r="C152" s="18"/>
+      <c r="D152" s="18"/>
+      <c r="E152" s="18"/>
       <c r="F152" s="6"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6">
       <c r="A153" s="1" t="s">
         <v>20</v>
       </c>
@@ -5120,7 +5413,7 @@
       </c>
       <c r="F153" s="5"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6">
       <c r="A154" s="2" t="s">
         <v>421</v>
       </c>
@@ -5138,7 +5431,7 @@
       </c>
       <c r="F154" s="5"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6">
       <c r="A155" s="2" t="s">
         <v>0</v>
       </c>
@@ -5156,7 +5449,7 @@
       </c>
       <c r="F155" s="5"/>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6">
       <c r="A156" s="2" t="s">
         <v>14</v>
       </c>
@@ -5173,17 +5466,17 @@
         <v>427</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A158" s="20" t="s">
+    <row r="158" spans="1:6" ht="15.6">
+      <c r="A158" s="18" t="s">
         <v>429</v>
       </c>
-      <c r="B158" s="20"/>
-      <c r="C158" s="20"/>
-      <c r="D158" s="20"/>
-      <c r="E158" s="20"/>
+      <c r="B158" s="18"/>
+      <c r="C158" s="18"/>
+      <c r="D158" s="18"/>
+      <c r="E158" s="18"/>
       <c r="F158" s="6"/>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6">
       <c r="A159" s="1" t="s">
         <v>20</v>
       </c>
@@ -5201,7 +5494,7 @@
       </c>
       <c r="F159" s="5"/>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6">
       <c r="A160" s="2" t="s">
         <v>430</v>
       </c>
@@ -5218,7 +5511,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6">
       <c r="A161" s="2" t="s">
         <v>421</v>
       </c>
@@ -5235,7 +5528,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" ht="28.8">
       <c r="A162" s="2" t="s">
         <v>435</v>
       </c>
@@ -5252,7 +5545,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6">
       <c r="A163" s="2" t="s">
         <v>14</v>
       </c>
@@ -5269,17 +5562,17 @@
         <v>438</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A165" s="20" t="s">
+    <row r="165" spans="1:6" ht="15.6">
+      <c r="A165" s="18" t="s">
         <v>439</v>
       </c>
-      <c r="B165" s="20"/>
-      <c r="C165" s="20"/>
-      <c r="D165" s="20"/>
-      <c r="E165" s="20"/>
+      <c r="B165" s="18"/>
+      <c r="C165" s="18"/>
+      <c r="D165" s="18"/>
+      <c r="E165" s="18"/>
       <c r="F165" s="6"/>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6">
       <c r="A166" s="1" t="s">
         <v>20</v>
       </c>
@@ -5297,7 +5590,7 @@
       </c>
       <c r="F166" s="5"/>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6">
       <c r="A167" s="2" t="s">
         <v>440</v>
       </c>
@@ -5314,7 +5607,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" ht="28.8">
       <c r="A168" s="2" t="s">
         <v>430</v>
       </c>
@@ -5331,7 +5624,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6">
       <c r="A169" s="2" t="s">
         <v>445</v>
       </c>
@@ -5348,7 +5641,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6">
       <c r="A170" s="2" t="s">
         <v>448</v>
       </c>
@@ -5365,7 +5658,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6">
       <c r="A171" s="2" t="s">
         <v>14</v>
       </c>
@@ -5382,41 +5675,41 @@
         <v>451</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6">
       <c r="A172" s="9"/>
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
       <c r="D172" s="9"/>
       <c r="E172" s="9"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6">
       <c r="A173" s="9"/>
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
       <c r="D173" s="9"/>
       <c r="E173" s="9"/>
     </row>
-    <row r="174" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A174" s="19" t="s">
+    <row r="174" spans="1:6" ht="18">
+      <c r="A174" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="B174" s="19"/>
-      <c r="C174" s="19"/>
-      <c r="D174" s="19"/>
-      <c r="E174" s="19"/>
-      <c r="F174" s="19"/>
-    </row>
-    <row r="176" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A176" s="16" t="s">
+      <c r="B174" s="17"/>
+      <c r="C174" s="17"/>
+      <c r="D174" s="17"/>
+      <c r="E174" s="17"/>
+      <c r="F174" s="17"/>
+    </row>
+    <row r="176" spans="1:6" ht="15.6">
+      <c r="A176" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="B176" s="17"/>
-      <c r="C176" s="17"/>
-      <c r="D176" s="17"/>
-      <c r="E176" s="17"/>
-      <c r="F176" s="18"/>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B176" s="15"/>
+      <c r="C176" s="15"/>
+      <c r="D176" s="15"/>
+      <c r="E176" s="15"/>
+      <c r="F176" s="16"/>
+    </row>
+    <row r="177" spans="1:9">
       <c r="A177" s="1" t="s">
         <v>20</v>
       </c>
@@ -5436,7 +5729,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9">
       <c r="A178" s="2" t="s">
         <v>258</v>
       </c>
@@ -5456,7 +5749,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" ht="43.2">
       <c r="A179" s="2" t="s">
         <v>86</v>
       </c>
@@ -5476,7 +5769,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" ht="43.2">
       <c r="A180" s="2" t="s">
         <v>266</v>
       </c>
@@ -5495,8 +5788,14 @@
       <c r="F180" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G180" s="22" t="s">
+        <v>753</v>
+      </c>
+      <c r="I180" s="23" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="115.2">
       <c r="A181" s="2" t="s">
         <v>271</v>
       </c>
@@ -5515,8 +5814,14 @@
       <c r="F181" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G181" s="22" t="s">
+        <v>754</v>
+      </c>
+      <c r="I181" s="23" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="28.8">
       <c r="A182" s="2" t="s">
         <v>276</v>
       </c>
@@ -5535,8 +5840,14 @@
       <c r="F182" s="2" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G182" t="s">
+        <v>755</v>
+      </c>
+      <c r="I182" s="23" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="28.8">
       <c r="A183" s="2" t="s">
         <v>135</v>
       </c>
@@ -5555,8 +5866,11 @@
       <c r="F183" s="2" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I183" s="23" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="28.8">
       <c r="A184" s="2" t="s">
         <v>90</v>
       </c>
@@ -5575,8 +5889,11 @@
       <c r="F184" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I184" s="23" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9">
       <c r="A185" s="2" t="s">
         <v>12</v>
       </c>
@@ -5595,8 +5912,11 @@
       <c r="F185" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I185" s="23" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="28.8">
       <c r="A186" s="2" t="s">
         <v>170</v>
       </c>
@@ -5615,8 +5935,11 @@
       <c r="F186" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G186" s="22" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9">
       <c r="A187" s="2" t="s">
         <v>16</v>
       </c>
@@ -5636,7 +5959,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" ht="28.8">
       <c r="A188" s="2" t="s">
         <v>14</v>
       </c>
@@ -5656,17 +5979,17 @@
         <v>270</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A190" s="16" t="s">
+    <row r="190" spans="1:9" ht="15.6">
+      <c r="A190" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="B190" s="17"/>
-      <c r="C190" s="17"/>
-      <c r="D190" s="17"/>
-      <c r="E190" s="17"/>
-      <c r="F190" s="18"/>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B190" s="15"/>
+      <c r="C190" s="15"/>
+      <c r="D190" s="15"/>
+      <c r="E190" s="15"/>
+      <c r="F190" s="16"/>
+    </row>
+    <row r="191" spans="1:9">
       <c r="A191" s="1" t="s">
         <v>20</v>
       </c>
@@ -5686,7 +6009,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9">
       <c r="A192" s="2" t="s">
         <v>141</v>
       </c>
@@ -5706,7 +6029,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" ht="28.8">
       <c r="A193" s="2" t="s">
         <v>258</v>
       </c>
@@ -5725,8 +6048,11 @@
       <c r="F193" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G193" s="24" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="28.8">
       <c r="A194" s="2" t="s">
         <v>131</v>
       </c>
@@ -5745,8 +6071,11 @@
       <c r="F194" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G194" s="23" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="43.2">
       <c r="A195" s="2" t="s">
         <v>305</v>
       </c>
@@ -5766,17 +6095,17 @@
         <v>308</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A197" s="16" t="s">
+    <row r="197" spans="1:8" ht="15.6">
+      <c r="A197" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="B197" s="17"/>
-      <c r="C197" s="17"/>
-      <c r="D197" s="17"/>
-      <c r="E197" s="17"/>
-      <c r="F197" s="18"/>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B197" s="15"/>
+      <c r="C197" s="15"/>
+      <c r="D197" s="15"/>
+      <c r="E197" s="15"/>
+      <c r="F197" s="16"/>
+    </row>
+    <row r="198" spans="1:8">
       <c r="A198" s="1" t="s">
         <v>20</v>
       </c>
@@ -5796,7 +6125,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8">
       <c r="A199" s="2" t="s">
         <v>326</v>
       </c>
@@ -5815,8 +6144,11 @@
       <c r="F199" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H199" s="24" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8">
       <c r="A200" s="2" t="s">
         <v>258</v>
       </c>
@@ -5835,8 +6167,11 @@
       <c r="F200" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H200" s="23" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" ht="28.8">
       <c r="A201" s="2" t="s">
         <v>156</v>
       </c>
@@ -5856,7 +6191,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" ht="28.8">
       <c r="A202" s="2" t="s">
         <v>315</v>
       </c>
@@ -5876,7 +6211,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" ht="28.8">
       <c r="A203" s="2" t="s">
         <v>319</v>
       </c>
@@ -5895,8 +6230,11 @@
       <c r="F203" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G203" s="22" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8">
       <c r="A204" s="2" t="s">
         <v>322</v>
       </c>
@@ -5916,27 +6254,27 @@
         <v>294</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A207" s="19" t="s">
+    <row r="207" spans="1:8" ht="18">
+      <c r="A207" s="17" t="s">
         <v>452</v>
       </c>
-      <c r="B207" s="19"/>
-      <c r="C207" s="19"/>
-      <c r="D207" s="19"/>
-      <c r="E207" s="19"/>
-      <c r="F207" s="19"/>
-    </row>
-    <row r="209" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A209" s="16" t="s">
+      <c r="B207" s="17"/>
+      <c r="C207" s="17"/>
+      <c r="D207" s="17"/>
+      <c r="E207" s="17"/>
+      <c r="F207" s="17"/>
+    </row>
+    <row r="209" spans="1:6" ht="15.6">
+      <c r="A209" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="B209" s="17"/>
-      <c r="C209" s="17"/>
-      <c r="D209" s="17"/>
-      <c r="E209" s="17"/>
-      <c r="F209" s="18"/>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B209" s="15"/>
+      <c r="C209" s="15"/>
+      <c r="D209" s="15"/>
+      <c r="E209" s="15"/>
+      <c r="F209" s="16"/>
+    </row>
+    <row r="210" spans="1:6">
       <c r="A210" s="1" t="s">
         <v>20</v>
       </c>
@@ -5956,7 +6294,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6">
       <c r="A211" s="2" t="s">
         <v>325</v>
       </c>
@@ -5974,7 +6312,7 @@
       </c>
       <c r="F211" s="2"/>
     </row>
-    <row r="212" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" ht="28.8">
       <c r="A212" s="2" t="s">
         <v>86</v>
       </c>
@@ -5992,7 +6330,7 @@
       </c>
       <c r="F212" s="2"/>
     </row>
-    <row r="213" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" ht="28.8">
       <c r="A213" s="2" t="s">
         <v>131</v>
       </c>
@@ -6010,7 +6348,7 @@
       </c>
       <c r="F213" s="2"/>
     </row>
-    <row r="214" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" ht="43.2">
       <c r="A214" s="2" t="s">
         <v>156</v>
       </c>
@@ -6030,7 +6368,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" ht="43.2">
       <c r="A215" s="2" t="s">
         <v>340</v>
       </c>
@@ -6048,7 +6386,7 @@
       </c>
       <c r="F215" s="2"/>
     </row>
-    <row r="216" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" ht="43.2">
       <c r="A216" s="2" t="s">
         <v>344</v>
       </c>
@@ -6066,7 +6404,7 @@
       </c>
       <c r="F216" s="2"/>
     </row>
-    <row r="217" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" ht="28.8">
       <c r="A217" s="2" t="s">
         <v>16</v>
       </c>
@@ -6084,7 +6422,7 @@
       </c>
       <c r="F217" s="2"/>
     </row>
-    <row r="218" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" ht="28.8">
       <c r="A218" s="2" t="s">
         <v>14</v>
       </c>
@@ -6102,27 +6440,27 @@
       </c>
       <c r="F218" s="2"/>
     </row>
-    <row r="221" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A221" s="19" t="s">
+    <row r="221" spans="1:6" ht="18">
+      <c r="A221" s="17" t="s">
         <v>453</v>
       </c>
-      <c r="B221" s="19"/>
-      <c r="C221" s="19"/>
-      <c r="D221" s="19"/>
-      <c r="E221" s="19"/>
-      <c r="F221" s="19"/>
-    </row>
-    <row r="223" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A223" s="16" t="s">
+      <c r="B221" s="17"/>
+      <c r="C221" s="17"/>
+      <c r="D221" s="17"/>
+      <c r="E221" s="17"/>
+      <c r="F221" s="17"/>
+    </row>
+    <row r="223" spans="1:6" ht="15.6">
+      <c r="A223" s="14" t="s">
         <v>352</v>
       </c>
-      <c r="B223" s="17"/>
-      <c r="C223" s="17"/>
-      <c r="D223" s="17"/>
-      <c r="E223" s="17"/>
-      <c r="F223" s="18"/>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B223" s="15"/>
+      <c r="C223" s="15"/>
+      <c r="D223" s="15"/>
+      <c r="E223" s="15"/>
+      <c r="F223" s="16"/>
+    </row>
+    <row r="224" spans="1:6">
       <c r="A224" s="1" t="s">
         <v>20</v>
       </c>
@@ -6142,7 +6480,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" ht="28.8">
       <c r="A225" s="2" t="s">
         <v>381</v>
       </c>
@@ -6160,7 +6498,7 @@
       </c>
       <c r="F225" s="2"/>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6">
       <c r="A226" s="2" t="s">
         <v>131</v>
       </c>
@@ -6178,7 +6516,7 @@
       </c>
       <c r="F226" s="2"/>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6">
       <c r="A227" s="2" t="s">
         <v>86</v>
       </c>
@@ -6196,7 +6534,7 @@
       </c>
       <c r="F227" s="2"/>
     </row>
-    <row r="228" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" ht="28.8">
       <c r="A228" s="2" t="s">
         <v>360</v>
       </c>
@@ -6214,7 +6552,7 @@
       </c>
       <c r="F228" s="2"/>
     </row>
-    <row r="229" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" ht="43.2">
       <c r="A229" s="2" t="s">
         <v>363</v>
       </c>
@@ -6234,7 +6572,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" ht="43.2">
       <c r="A230" s="2" t="s">
         <v>368</v>
       </c>
@@ -6252,7 +6590,7 @@
       </c>
       <c r="F230" s="2"/>
     </row>
-    <row r="231" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" ht="28.8">
       <c r="A231" s="2" t="s">
         <v>371</v>
       </c>
@@ -6270,7 +6608,7 @@
       </c>
       <c r="F231" s="2"/>
     </row>
-    <row r="232" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" ht="28.8">
       <c r="A232" s="2" t="s">
         <v>374</v>
       </c>
@@ -6288,7 +6626,7 @@
       </c>
       <c r="F232" s="2"/>
     </row>
-    <row r="233" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" ht="28.8">
       <c r="A233" s="2" t="s">
         <v>90</v>
       </c>
@@ -6306,7 +6644,7 @@
       </c>
       <c r="F233" s="2"/>
     </row>
-    <row r="234" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" ht="28.8">
       <c r="A234" s="2" t="s">
         <v>16</v>
       </c>
@@ -6324,7 +6662,7 @@
       </c>
       <c r="F234" s="2"/>
     </row>
-    <row r="235" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" ht="28.8">
       <c r="A235" s="2" t="s">
         <v>14</v>
       </c>
@@ -6342,17 +6680,17 @@
       </c>
       <c r="F235" s="2"/>
     </row>
-    <row r="237" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A237" s="16" t="s">
+    <row r="237" spans="1:6" ht="15.6">
+      <c r="A237" s="14" t="s">
         <v>395</v>
       </c>
-      <c r="B237" s="17"/>
-      <c r="C237" s="17"/>
-      <c r="D237" s="17"/>
-      <c r="E237" s="18"/>
+      <c r="B237" s="15"/>
+      <c r="C237" s="15"/>
+      <c r="D237" s="15"/>
+      <c r="E237" s="16"/>
       <c r="F237" s="6"/>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6">
       <c r="A238" s="1" t="s">
         <v>20</v>
       </c>
@@ -6370,7 +6708,7 @@
       </c>
       <c r="F238" s="5"/>
     </row>
-    <row r="239" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" ht="28.8">
       <c r="A239" s="2" t="s">
         <v>381</v>
       </c>
@@ -6388,7 +6726,7 @@
       </c>
       <c r="F239" s="9"/>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6">
       <c r="A240" s="2" t="s">
         <v>133</v>
       </c>
@@ -6406,7 +6744,7 @@
       </c>
       <c r="F240" s="9"/>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6">
       <c r="A241" s="2" t="s">
         <v>86</v>
       </c>
@@ -6424,7 +6762,7 @@
       </c>
       <c r="F241" s="9"/>
     </row>
-    <row r="242" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" ht="28.8">
       <c r="A242" s="2" t="s">
         <v>388</v>
       </c>
@@ -6442,7 +6780,7 @@
       </c>
       <c r="F242" s="9"/>
     </row>
-    <row r="243" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:6" ht="28.8">
       <c r="A243" s="2" t="s">
         <v>391</v>
       </c>
@@ -6460,7 +6798,7 @@
       </c>
       <c r="F243" s="9"/>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6">
       <c r="A244" s="2" t="s">
         <v>90</v>
       </c>
@@ -6478,7 +6816,7 @@
       </c>
       <c r="F244" s="9"/>
     </row>
-    <row r="245" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" ht="28.8">
       <c r="A245" s="2" t="s">
         <v>16</v>
       </c>
@@ -6496,7 +6834,7 @@
       </c>
       <c r="F245" s="9"/>
     </row>
-    <row r="246" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" ht="28.8">
       <c r="A246" s="2" t="s">
         <v>14</v>
       </c>
@@ -6514,20 +6852,20 @@
       </c>
       <c r="F246" s="9"/>
     </row>
-    <row r="247" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" ht="18">
       <c r="A247" s="7"/>
     </row>
-    <row r="248" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A248" s="20" t="s">
+    <row r="248" spans="1:6" ht="15.6">
+      <c r="A248" s="18" t="s">
         <v>416</v>
       </c>
-      <c r="B248" s="20"/>
-      <c r="C248" s="20"/>
-      <c r="D248" s="20"/>
-      <c r="E248" s="20"/>
-      <c r="F248" s="20"/>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B248" s="18"/>
+      <c r="C248" s="18"/>
+      <c r="D248" s="18"/>
+      <c r="E248" s="18"/>
+      <c r="F248" s="18"/>
+    </row>
+    <row r="249" spans="1:6">
       <c r="A249" s="1" t="s">
         <v>353</v>
       </c>
@@ -6547,7 +6885,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" ht="28.8">
       <c r="A250" s="2" t="s">
         <v>329</v>
       </c>
@@ -6565,7 +6903,7 @@
       </c>
       <c r="F250" s="2"/>
     </row>
-    <row r="251" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" ht="28.8">
       <c r="A251" s="2" t="s">
         <v>86</v>
       </c>
@@ -6583,7 +6921,7 @@
       </c>
       <c r="F251" s="2"/>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6">
       <c r="A252" s="2" t="s">
         <v>131</v>
       </c>
@@ -6601,7 +6939,7 @@
       </c>
       <c r="F252" s="2"/>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6">
       <c r="A253" s="2" t="s">
         <v>133</v>
       </c>
@@ -6619,7 +6957,7 @@
       </c>
       <c r="F253" s="2"/>
     </row>
-    <row r="254" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" ht="28.8">
       <c r="A254" s="2" t="s">
         <v>360</v>
       </c>
@@ -6637,7 +6975,7 @@
       </c>
       <c r="F254" s="2"/>
     </row>
-    <row r="255" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" ht="28.8">
       <c r="A255" s="2" t="s">
         <v>363</v>
       </c>
@@ -6655,7 +6993,7 @@
       </c>
       <c r="F255" s="2"/>
     </row>
-    <row r="256" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" ht="28.8">
       <c r="A256" s="2" t="s">
         <v>405</v>
       </c>
@@ -6673,7 +7011,7 @@
       </c>
       <c r="F256" s="2"/>
     </row>
-    <row r="257" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" ht="28.8">
       <c r="A257" s="2" t="s">
         <v>408</v>
       </c>
@@ -6691,7 +7029,7 @@
       </c>
       <c r="F257" s="2"/>
     </row>
-    <row r="258" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" ht="28.8">
       <c r="A258" s="2" t="s">
         <v>411</v>
       </c>
@@ -6711,7 +7049,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:6">
       <c r="A259" s="2" t="s">
         <v>90</v>
       </c>
@@ -6729,7 +7067,7 @@
       </c>
       <c r="F259" s="2"/>
     </row>
-    <row r="260" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" ht="28.8">
       <c r="A260" s="2" t="s">
         <v>16</v>
       </c>
@@ -6747,7 +7085,7 @@
       </c>
       <c r="F260" s="2"/>
     </row>
-    <row r="261" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" ht="28.8">
       <c r="A261" s="2" t="s">
         <v>14</v>
       </c>
@@ -6765,17 +7103,17 @@
       </c>
       <c r="F261" s="2"/>
     </row>
-    <row r="263" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A263" s="20" t="s">
+    <row r="263" spans="1:6" ht="15.6">
+      <c r="A263" s="18" t="s">
         <v>633</v>
       </c>
-      <c r="B263" s="20"/>
-      <c r="C263" s="20"/>
-      <c r="D263" s="20"/>
-      <c r="E263" s="20"/>
-      <c r="F263" s="20"/>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B263" s="18"/>
+      <c r="C263" s="18"/>
+      <c r="D263" s="18"/>
+      <c r="E263" s="18"/>
+      <c r="F263" s="18"/>
+    </row>
+    <row r="264" spans="1:6">
       <c r="A264" s="1" t="s">
         <v>20</v>
       </c>
@@ -6795,7 +7133,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6">
       <c r="A265" s="2" t="s">
         <v>624</v>
       </c>
@@ -6813,7 +7151,7 @@
       </c>
       <c r="F265" s="2"/>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6">
       <c r="A266" s="2" t="s">
         <v>191</v>
       </c>
@@ -6833,7 +7171,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6">
       <c r="A267" s="2" t="s">
         <v>195</v>
       </c>
@@ -6851,7 +7189,7 @@
       </c>
       <c r="F267" s="2"/>
     </row>
-    <row r="268" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" ht="28.8">
       <c r="A268" s="2" t="s">
         <v>86</v>
       </c>
@@ -6869,7 +7207,7 @@
       </c>
       <c r="F268" s="2"/>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6">
       <c r="A269" s="2" t="s">
         <v>131</v>
       </c>
@@ -6887,7 +7225,7 @@
       </c>
       <c r="F269" s="2"/>
     </row>
-    <row r="270" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" ht="28.8">
       <c r="A270" s="2" t="s">
         <v>133</v>
       </c>
@@ -6907,7 +7245,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="271" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" ht="28.8">
       <c r="A271" s="2" t="s">
         <v>138</v>
       </c>
@@ -6927,7 +7265,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="272" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" ht="28.8">
       <c r="A272" s="2" t="s">
         <v>626</v>
       </c>
@@ -6945,7 +7283,7 @@
       </c>
       <c r="F272" s="2"/>
     </row>
-    <row r="273" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" ht="28.8">
       <c r="A273" s="2" t="s">
         <v>627</v>
       </c>
@@ -6965,7 +7303,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="274" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" ht="28.8">
       <c r="A274" s="2" t="s">
         <v>629</v>
       </c>
@@ -6985,7 +7323,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="275" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" ht="28.8">
       <c r="A275" s="2" t="s">
         <v>16</v>
       </c>
@@ -7003,7 +7341,7 @@
       </c>
       <c r="F275" s="2"/>
     </row>
-    <row r="276" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" ht="28.8">
       <c r="A276" s="2" t="s">
         <v>631</v>
       </c>
@@ -7021,36 +7359,36 @@
       </c>
       <c r="F276" s="2"/>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6">
       <c r="A277" s="9"/>
       <c r="B277" s="9"/>
       <c r="C277" s="9"/>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6">
       <c r="A278" s="9"/>
       <c r="B278" s="9"/>
       <c r="C278" s="9"/>
     </row>
-    <row r="279" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A279" s="19" t="s">
+    <row r="279" spans="1:6" ht="18">
+      <c r="A279" s="17" t="s">
         <v>454</v>
       </c>
-      <c r="B279" s="19"/>
-      <c r="C279" s="19"/>
-      <c r="D279" s="19"/>
-      <c r="E279" s="19"/>
-      <c r="F279" s="19"/>
-    </row>
-    <row r="281" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A281" s="16" t="s">
+      <c r="B279" s="17"/>
+      <c r="C279" s="17"/>
+      <c r="D279" s="17"/>
+      <c r="E279" s="17"/>
+      <c r="F279" s="17"/>
+    </row>
+    <row r="281" spans="1:6" ht="15.6">
+      <c r="A281" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="B281" s="17"/>
-      <c r="C281" s="17"/>
-      <c r="D281" s="17"/>
-      <c r="E281" s="18"/>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B281" s="15"/>
+      <c r="C281" s="15"/>
+      <c r="D281" s="15"/>
+      <c r="E281" s="16"/>
+    </row>
+    <row r="282" spans="1:6">
       <c r="A282" s="1" t="s">
         <v>20</v>
       </c>
@@ -7068,7 +7406,7 @@
       </c>
       <c r="F282" s="5"/>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6">
       <c r="A283" s="2" t="s">
         <v>253</v>
       </c>
@@ -7086,7 +7424,7 @@
       </c>
       <c r="F283" s="5"/>
     </row>
-    <row r="284" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" ht="28.8">
       <c r="A284" s="2" t="s">
         <v>86</v>
       </c>
@@ -7104,7 +7442,7 @@
       </c>
       <c r="F284" s="5"/>
     </row>
-    <row r="285" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" ht="43.2">
       <c r="A285" s="2" t="s">
         <v>90</v>
       </c>
@@ -7122,7 +7460,7 @@
       </c>
       <c r="F285" s="5"/>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:6">
       <c r="A286" s="2" t="s">
         <v>165</v>
       </c>
@@ -7140,7 +7478,7 @@
       </c>
       <c r="F286" s="5"/>
     </row>
-    <row r="287" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" ht="43.2">
       <c r="A287" s="2" t="s">
         <v>170</v>
       </c>
@@ -7158,7 +7496,7 @@
       </c>
       <c r="F287" s="5"/>
     </row>
-    <row r="288" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" ht="28.8">
       <c r="A288" s="2" t="s">
         <v>173</v>
       </c>
@@ -7175,7 +7513,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="289" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" ht="28.8">
       <c r="A289" s="2" t="s">
         <v>177</v>
       </c>
@@ -7192,7 +7530,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6">
       <c r="A290" s="2" t="s">
         <v>180</v>
       </c>
@@ -7209,7 +7547,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6">
       <c r="A291" s="2" t="s">
         <v>14</v>
       </c>
@@ -7226,7 +7564,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" ht="28.8">
       <c r="A292" s="2" t="s">
         <v>16</v>
       </c>
@@ -7243,41 +7581,41 @@
         <v>100</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:6">
       <c r="A293" s="9"/>
       <c r="B293" s="9"/>
       <c r="C293" s="9"/>
       <c r="D293" s="9"/>
       <c r="E293" s="9"/>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6">
       <c r="A294" s="9"/>
       <c r="B294" s="9"/>
       <c r="C294" s="9"/>
       <c r="D294" s="9"/>
       <c r="E294" s="9"/>
     </row>
-    <row r="295" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A295" s="19" t="s">
+    <row r="295" spans="1:6" ht="18">
+      <c r="A295" s="17" t="s">
         <v>455</v>
       </c>
-      <c r="B295" s="19"/>
-      <c r="C295" s="19"/>
-      <c r="D295" s="19"/>
-      <c r="E295" s="19"/>
-      <c r="F295" s="19"/>
-    </row>
-    <row r="297" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A297" s="16" t="s">
+      <c r="B295" s="17"/>
+      <c r="C295" s="17"/>
+      <c r="D295" s="17"/>
+      <c r="E295" s="17"/>
+      <c r="F295" s="17"/>
+    </row>
+    <row r="297" spans="1:6" ht="15.6">
+      <c r="A297" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="B297" s="17"/>
-      <c r="C297" s="17"/>
-      <c r="D297" s="17"/>
-      <c r="E297" s="18"/>
+      <c r="B297" s="15"/>
+      <c r="C297" s="15"/>
+      <c r="D297" s="15"/>
+      <c r="E297" s="16"/>
       <c r="F297" s="6"/>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6">
       <c r="A298" s="1" t="s">
         <v>20</v>
       </c>
@@ -7295,7 +7633,7 @@
       </c>
       <c r="F298" s="5"/>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6">
       <c r="A299" s="2" t="s">
         <v>210</v>
       </c>
@@ -7312,7 +7650,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6">
       <c r="A300" s="2" t="s">
         <v>188</v>
       </c>
@@ -7329,7 +7667,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:6" ht="28.8">
       <c r="A301" s="2" t="s">
         <v>191</v>
       </c>
@@ -7346,7 +7684,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6">
       <c r="A302" s="2" t="s">
         <v>195</v>
       </c>
@@ -7363,7 +7701,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="303" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:6" ht="28.8">
       <c r="A303" s="2" t="s">
         <v>14</v>
       </c>
@@ -7380,7 +7718,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="304" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" ht="28.8">
       <c r="A304" s="2" t="s">
         <v>16</v>
       </c>
@@ -7397,16 +7735,16 @@
         <v>202</v>
       </c>
     </row>
-    <row r="306" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A306" s="16" t="s">
+    <row r="306" spans="1:5" ht="15.6">
+      <c r="A306" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="B306" s="17"/>
-      <c r="C306" s="17"/>
-      <c r="D306" s="17"/>
-      <c r="E306" s="18"/>
-    </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B306" s="15"/>
+      <c r="C306" s="15"/>
+      <c r="D306" s="15"/>
+      <c r="E306" s="16"/>
+    </row>
+    <row r="307" spans="1:5">
       <c r="A307" s="1" t="s">
         <v>20</v>
       </c>
@@ -7423,7 +7761,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5">
       <c r="A308" s="2" t="s">
         <v>214</v>
       </c>
@@ -7440,7 +7778,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="309" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" ht="28.8">
       <c r="A309" s="2" t="s">
         <v>0</v>
       </c>
@@ -7457,7 +7795,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="310" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" ht="28.8">
       <c r="A310" s="2" t="s">
         <v>14</v>
       </c>
@@ -7474,23 +7812,23 @@
         <v>207</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5">
       <c r="A311" s="3"/>
       <c r="B311" s="3"/>
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
       <c r="E311" s="3"/>
     </row>
-    <row r="312" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A312" s="16" t="s">
+    <row r="312" spans="1:5" ht="15.6">
+      <c r="A312" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="B312" s="17"/>
-      <c r="C312" s="17"/>
-      <c r="D312" s="17"/>
-      <c r="E312" s="18"/>
-    </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B312" s="15"/>
+      <c r="C312" s="15"/>
+      <c r="D312" s="15"/>
+      <c r="E312" s="16"/>
+    </row>
+    <row r="313" spans="1:5">
       <c r="A313" s="1" t="s">
         <v>20</v>
       </c>
@@ -7507,7 +7845,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5">
       <c r="A314" s="2" t="s">
         <v>243</v>
       </c>
@@ -7524,7 +7862,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5">
       <c r="A315" s="2" t="s">
         <v>210</v>
       </c>
@@ -7541,7 +7879,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5">
       <c r="A316" s="2" t="s">
         <v>214</v>
       </c>
@@ -7558,7 +7896,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5">
       <c r="A317" s="2" t="s">
         <v>218</v>
       </c>
@@ -7575,7 +7913,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="318" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" ht="28.8">
       <c r="A318" s="2" t="s">
         <v>14</v>
       </c>
@@ -7592,7 +7930,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="319" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" ht="28.8">
       <c r="A319" s="2" t="s">
         <v>16</v>
       </c>
@@ -7609,16 +7947,16 @@
         <v>202</v>
       </c>
     </row>
-    <row r="321" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A321" s="16" t="s">
+    <row r="321" spans="1:5" ht="15.6">
+      <c r="A321" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="B321" s="17"/>
-      <c r="C321" s="17"/>
-      <c r="D321" s="17"/>
-      <c r="E321" s="18"/>
-    </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B321" s="15"/>
+      <c r="C321" s="15"/>
+      <c r="D321" s="15"/>
+      <c r="E321" s="16"/>
+    </row>
+    <row r="322" spans="1:5">
       <c r="A322" s="1" t="s">
         <v>20</v>
       </c>
@@ -7635,7 +7973,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5">
       <c r="A323" s="2" t="s">
         <v>255</v>
       </c>
@@ -7652,7 +7990,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="324" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" ht="28.8">
       <c r="A324" s="2" t="s">
         <v>225</v>
       </c>
@@ -7669,7 +8007,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5">
       <c r="A325" s="2" t="s">
         <v>210</v>
       </c>
@@ -7686,7 +8024,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="326" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" ht="28.8">
       <c r="A326" s="2" t="s">
         <v>231</v>
       </c>
@@ -7703,7 +8041,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="327" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" ht="28.8">
       <c r="A327" s="2" t="s">
         <v>16</v>
       </c>
@@ -7720,16 +8058,16 @@
         <v>202</v>
       </c>
     </row>
-    <row r="329" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A329" s="20" t="s">
+    <row r="329" spans="1:5" ht="15.6">
+      <c r="A329" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="B329" s="20"/>
-      <c r="C329" s="20"/>
-      <c r="D329" s="20"/>
-      <c r="E329" s="20"/>
-    </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B329" s="18"/>
+      <c r="C329" s="18"/>
+      <c r="D329" s="18"/>
+      <c r="E329" s="18"/>
+    </row>
+    <row r="330" spans="1:5">
       <c r="A330" s="1" t="s">
         <v>20</v>
       </c>
@@ -7746,7 +8084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5">
       <c r="A331" s="2" t="s">
         <v>257</v>
       </c>
@@ -7763,7 +8101,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="332" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" ht="28.8">
       <c r="A332" s="2" t="s">
         <v>225</v>
       </c>
@@ -7780,7 +8118,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5">
       <c r="A333" s="2" t="s">
         <v>210</v>
       </c>
@@ -7797,7 +8135,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5">
       <c r="A334" s="2" t="s">
         <v>243</v>
       </c>
@@ -7814,7 +8152,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="335" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" ht="28.8">
       <c r="A335" s="2" t="s">
         <v>247</v>
       </c>
@@ -7831,7 +8169,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="336" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" ht="28.8">
       <c r="A336" s="2" t="s">
         <v>16</v>
       </c>
@@ -7848,41 +8186,41 @@
         <v>251</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:6">
       <c r="A337" s="9"/>
       <c r="B337" s="9"/>
       <c r="C337" s="9"/>
       <c r="D337" s="9"/>
       <c r="E337" s="9"/>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:6">
       <c r="A338" s="9"/>
       <c r="B338" s="9"/>
       <c r="C338" s="9"/>
       <c r="D338" s="9"/>
       <c r="E338" s="9"/>
     </row>
-    <row r="339" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A339" s="19" t="s">
+    <row r="339" spans="1:6" ht="18">
+      <c r="A339" s="17" t="s">
         <v>456</v>
       </c>
-      <c r="B339" s="19"/>
-      <c r="C339" s="19"/>
-      <c r="D339" s="19"/>
-      <c r="E339" s="19"/>
-      <c r="F339" s="19"/>
-    </row>
-    <row r="341" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A341" s="20" t="s">
+      <c r="B339" s="17"/>
+      <c r="C339" s="17"/>
+      <c r="D339" s="17"/>
+      <c r="E339" s="17"/>
+      <c r="F339" s="17"/>
+    </row>
+    <row r="341" spans="1:6" ht="15.6">
+      <c r="A341" s="18" t="s">
         <v>457</v>
       </c>
-      <c r="B341" s="20"/>
-      <c r="C341" s="20"/>
-      <c r="D341" s="20"/>
-      <c r="E341" s="20"/>
-      <c r="F341" s="20"/>
-    </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B341" s="18"/>
+      <c r="C341" s="18"/>
+      <c r="D341" s="18"/>
+      <c r="E341" s="18"/>
+      <c r="F341" s="18"/>
+    </row>
+    <row r="342" spans="1:6">
       <c r="A342" s="1" t="s">
         <v>20</v>
       </c>
@@ -7902,7 +8240,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:6">
       <c r="A343" s="2" t="s">
         <v>210</v>
       </c>
@@ -7922,7 +8260,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="344" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:6" ht="28.8">
       <c r="A344" s="2" t="s">
         <v>458</v>
       </c>
@@ -7940,7 +8278,7 @@
       </c>
       <c r="F344" s="2"/>
     </row>
-    <row r="345" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:6" ht="28.8">
       <c r="A345" s="2" t="s">
         <v>459</v>
       </c>
@@ -7960,7 +8298,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:6">
       <c r="A346" s="2" t="s">
         <v>90</v>
       </c>
@@ -7978,7 +8316,7 @@
       </c>
       <c r="F346" s="2"/>
     </row>
-    <row r="347" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:6" ht="28.8">
       <c r="A347" s="2" t="s">
         <v>12</v>
       </c>
@@ -7996,7 +8334,7 @@
       </c>
       <c r="F347" s="2"/>
     </row>
-    <row r="348" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:6" ht="28.8">
       <c r="A348" s="2" t="s">
         <v>86</v>
       </c>
@@ -8016,7 +8354,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:6">
       <c r="A349" s="2" t="s">
         <v>468</v>
       </c>
@@ -8034,7 +8372,7 @@
       </c>
       <c r="F349" s="2"/>
     </row>
-    <row r="350" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:6" ht="28.8">
       <c r="A350" s="2" t="s">
         <v>14</v>
       </c>
@@ -8052,20 +8390,20 @@
       </c>
       <c r="F350" s="2"/>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:6">
       <c r="F351" s="9"/>
     </row>
-    <row r="352" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A352" s="20" t="s">
+    <row r="352" spans="1:6" ht="15.6">
+      <c r="A352" s="18" t="s">
         <v>500</v>
       </c>
-      <c r="B352" s="20"/>
-      <c r="C352" s="20"/>
-      <c r="D352" s="20"/>
-      <c r="E352" s="20"/>
-      <c r="F352" s="20"/>
-    </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B352" s="18"/>
+      <c r="C352" s="18"/>
+      <c r="D352" s="18"/>
+      <c r="E352" s="18"/>
+      <c r="F352" s="18"/>
+    </row>
+    <row r="353" spans="1:6">
       <c r="A353" s="1" t="s">
         <v>20</v>
       </c>
@@ -8085,7 +8423,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:6">
       <c r="A354" s="2" t="s">
         <v>243</v>
       </c>
@@ -8105,7 +8443,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:6">
       <c r="A355" s="2" t="s">
         <v>210</v>
       </c>
@@ -8123,7 +8461,7 @@
       </c>
       <c r="F355" s="10"/>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:6">
       <c r="A356" s="2" t="s">
         <v>218</v>
       </c>
@@ -8141,7 +8479,7 @@
       </c>
       <c r="F356" s="2"/>
     </row>
-    <row r="357" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:6" ht="28.8">
       <c r="A357" s="2" t="s">
         <v>131</v>
       </c>
@@ -8159,7 +8497,7 @@
       </c>
       <c r="F357" s="2"/>
     </row>
-    <row r="358" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:6" ht="28.8">
       <c r="A358" s="2" t="s">
         <v>133</v>
       </c>
@@ -8177,7 +8515,7 @@
       </c>
       <c r="F358" s="2"/>
     </row>
-    <row r="359" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:6" ht="28.8">
       <c r="A359" s="2" t="s">
         <v>14</v>
       </c>
@@ -8195,7 +8533,7 @@
       </c>
       <c r="F359" s="2"/>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:6">
       <c r="A360" s="9"/>
       <c r="B360" s="9"/>
       <c r="C360" s="9"/>
@@ -8203,17 +8541,17 @@
       <c r="E360" s="9"/>
       <c r="F360" s="9"/>
     </row>
-    <row r="361" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A361" s="20" t="s">
+    <row r="361" spans="1:6" ht="15.6">
+      <c r="A361" s="18" t="s">
         <v>488</v>
       </c>
-      <c r="B361" s="20"/>
-      <c r="C361" s="20"/>
-      <c r="D361" s="20"/>
-      <c r="E361" s="20"/>
-      <c r="F361" s="20"/>
-    </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B361" s="18"/>
+      <c r="C361" s="18"/>
+      <c r="D361" s="18"/>
+      <c r="E361" s="18"/>
+      <c r="F361" s="18"/>
+    </row>
+    <row r="362" spans="1:6">
       <c r="A362" s="1" t="s">
         <v>20</v>
       </c>
@@ -8233,7 +8571,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:6">
       <c r="A363" s="2" t="s">
         <v>257</v>
       </c>
@@ -8253,7 +8591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="364" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:6" ht="28.8">
       <c r="A364" s="2" t="s">
         <v>210</v>
       </c>
@@ -8271,7 +8609,7 @@
       </c>
       <c r="F364" s="10"/>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:6">
       <c r="A365" s="2" t="s">
         <v>243</v>
       </c>
@@ -8289,7 +8627,7 @@
       </c>
       <c r="F365" s="10"/>
     </row>
-    <row r="366" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:6" ht="28.8">
       <c r="A366" s="2" t="s">
         <v>156</v>
       </c>
@@ -8307,7 +8645,7 @@
       </c>
       <c r="F366" s="2"/>
     </row>
-    <row r="367" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:6" ht="28.8">
       <c r="A367" s="2" t="s">
         <v>82</v>
       </c>
@@ -8325,7 +8663,7 @@
       </c>
       <c r="F367" s="2"/>
     </row>
-    <row r="368" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:6" ht="28.8">
       <c r="A368" s="2" t="s">
         <v>247</v>
       </c>
@@ -8343,7 +8681,7 @@
       </c>
       <c r="F368" s="2"/>
     </row>
-    <row r="369" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:6" ht="28.8">
       <c r="A369" s="2" t="s">
         <v>486</v>
       </c>
@@ -8361,20 +8699,20 @@
       </c>
       <c r="F369" s="2"/>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:6">
       <c r="F370" s="9"/>
     </row>
-    <row r="371" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A371" s="15" t="s">
+    <row r="371" spans="1:6" ht="15.6">
+      <c r="A371" s="20" t="s">
         <v>750</v>
       </c>
-      <c r="B371" s="15"/>
-      <c r="C371" s="15"/>
-      <c r="D371" s="15"/>
-      <c r="E371" s="15"/>
-      <c r="F371" s="15"/>
-    </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B371" s="20"/>
+      <c r="C371" s="20"/>
+      <c r="D371" s="20"/>
+      <c r="E371" s="20"/>
+      <c r="F371" s="20"/>
+    </row>
+    <row r="372" spans="1:6">
       <c r="A372" s="1" t="s">
         <v>20</v>
       </c>
@@ -8394,7 +8732,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:6">
       <c r="A373" s="2" t="s">
         <v>740</v>
       </c>
@@ -8412,7 +8750,7 @@
       </c>
       <c r="F373" s="2"/>
     </row>
-    <row r="374" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:6" ht="28.8">
       <c r="A374" s="2" t="s">
         <v>210</v>
       </c>
@@ -8430,7 +8768,7 @@
       </c>
       <c r="F374" s="2"/>
     </row>
-    <row r="375" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:6" ht="57.6">
       <c r="A375" s="2" t="s">
         <v>744</v>
       </c>
@@ -8450,7 +8788,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="376" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:6" ht="28.8">
       <c r="A376" s="2" t="s">
         <v>486</v>
       </c>
@@ -8468,32 +8806,32 @@
       </c>
       <c r="F376" s="2"/>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:6">
       <c r="F377" s="9"/>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:6">
       <c r="F378" s="9"/>
     </row>
-    <row r="379" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A379" s="19" t="s">
+    <row r="379" spans="1:6" ht="18">
+      <c r="A379" s="17" t="s">
         <v>575</v>
       </c>
-      <c r="B379" s="19"/>
-      <c r="C379" s="19"/>
-      <c r="D379" s="19"/>
-      <c r="E379" s="19"/>
-      <c r="F379" s="19"/>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A381" s="21" t="s">
+      <c r="B379" s="17"/>
+      <c r="C379" s="17"/>
+      <c r="D379" s="17"/>
+      <c r="E379" s="17"/>
+      <c r="F379" s="17"/>
+    </row>
+    <row r="381" spans="1:6">
+      <c r="A381" s="19" t="s">
         <v>621</v>
       </c>
-      <c r="B381" s="21"/>
-      <c r="C381" s="21"/>
-      <c r="D381" s="21"/>
-      <c r="E381" s="21"/>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B381" s="19"/>
+      <c r="C381" s="19"/>
+      <c r="D381" s="19"/>
+      <c r="E381" s="19"/>
+    </row>
+    <row r="382" spans="1:6">
       <c r="A382" s="11" t="s">
         <v>20</v>
       </c>
@@ -8510,7 +8848,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="383" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:6" ht="28.8">
       <c r="A383" s="10" t="s">
         <v>577</v>
       </c>
@@ -8527,7 +8865,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="384" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:6" ht="43.2">
       <c r="A384" s="10" t="s">
         <v>86</v>
       </c>
@@ -8544,7 +8882,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="385" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:5" ht="28.8">
       <c r="A385" s="10" t="s">
         <v>82</v>
       </c>
@@ -8561,7 +8899,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:5">
       <c r="A386" s="10" t="s">
         <v>9</v>
       </c>
@@ -8578,7 +8916,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:5">
       <c r="A387" s="10" t="s">
         <v>114</v>
       </c>
@@ -8595,7 +8933,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:5">
       <c r="A388" s="10" t="s">
         <v>90</v>
       </c>
@@ -8612,7 +8950,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:5">
       <c r="A389" s="10" t="s">
         <v>12</v>
       </c>
@@ -8629,7 +8967,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="390" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:5" ht="28.8">
       <c r="A390" s="10" t="s">
         <v>14</v>
       </c>
@@ -8646,7 +8984,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:5">
       <c r="A391" s="10" t="s">
         <v>16</v>
       </c>
@@ -8663,7 +9001,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:5">
       <c r="A392" s="10" t="s">
         <v>501</v>
       </c>
@@ -8680,16 +9018,16 @@
         <v>505</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A395" s="21" t="s">
+    <row r="395" spans="1:5">
+      <c r="A395" s="19" t="s">
         <v>622</v>
       </c>
-      <c r="B395" s="21"/>
-      <c r="C395" s="21"/>
-      <c r="D395" s="21"/>
-      <c r="E395" s="21"/>
-    </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B395" s="19"/>
+      <c r="C395" s="19"/>
+      <c r="D395" s="19"/>
+      <c r="E395" s="19"/>
+    </row>
+    <row r="396" spans="1:5">
       <c r="A396" s="11" t="s">
         <v>20</v>
       </c>
@@ -8706,7 +9044,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="397" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:5" ht="28.8">
       <c r="A397" s="10" t="s">
         <v>591</v>
       </c>
@@ -8723,7 +9061,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="398" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:5" ht="28.8">
       <c r="A398" s="10" t="s">
         <v>577</v>
       </c>
@@ -8740,7 +9078,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:5">
       <c r="A399" s="10" t="s">
         <v>596</v>
       </c>
@@ -8757,7 +9095,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:5">
       <c r="A400" s="10" t="s">
         <v>599</v>
       </c>
@@ -8774,7 +9112,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:6">
       <c r="A401" s="10" t="s">
         <v>604</v>
       </c>
@@ -8791,7 +9129,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="402" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:6" ht="28.8">
       <c r="A402" s="10" t="s">
         <v>607</v>
       </c>
@@ -8808,7 +9146,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:6">
       <c r="A403" s="10" t="s">
         <v>610</v>
       </c>
@@ -8825,7 +9163,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="404" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:6" ht="28.8">
       <c r="A404" s="10" t="s">
         <v>131</v>
       </c>
@@ -8842,7 +9180,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:6">
       <c r="A405" s="10" t="s">
         <v>616</v>
       </c>
@@ -8859,7 +9197,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:6">
       <c r="A406" s="10" t="s">
         <v>411</v>
       </c>
@@ -8876,7 +9214,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:6">
       <c r="A407" s="10" t="s">
         <v>16</v>
       </c>
@@ -8893,7 +9231,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:6">
       <c r="A408" s="10" t="s">
         <v>501</v>
       </c>
@@ -8910,32 +9248,32 @@
         <v>505</v>
       </c>
     </row>
-    <row r="411" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A411" s="19" t="s">
+    <row r="411" spans="1:6" ht="18">
+      <c r="A411" s="17" t="s">
         <v>700</v>
       </c>
-      <c r="B411" s="19"/>
-      <c r="C411" s="19"/>
-      <c r="D411" s="19"/>
-      <c r="E411" s="19"/>
-      <c r="F411" s="19"/>
-    </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B411" s="17"/>
+      <c r="C411" s="17"/>
+      <c r="D411" s="17"/>
+      <c r="E411" s="17"/>
+      <c r="F411" s="17"/>
+    </row>
+    <row r="412" spans="1:6">
       <c r="B412" s="9"/>
       <c r="C412" s="9"/>
       <c r="D412" s="9"/>
     </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A413" s="21" t="s">
+    <row r="413" spans="1:6">
+      <c r="A413" s="19" t="s">
         <v>701</v>
       </c>
-      <c r="B413" s="21"/>
-      <c r="C413" s="21"/>
-      <c r="D413" s="21"/>
-      <c r="E413" s="21"/>
-      <c r="F413" s="21"/>
-    </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B413" s="19"/>
+      <c r="C413" s="19"/>
+      <c r="D413" s="19"/>
+      <c r="E413" s="19"/>
+      <c r="F413" s="19"/>
+    </row>
+    <row r="414" spans="1:6">
       <c r="A414" s="1" t="s">
         <v>353</v>
       </c>
@@ -8955,7 +9293,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="415" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:6" ht="28.8">
       <c r="A415" s="2" t="s">
         <v>657</v>
       </c>
@@ -8975,7 +9313,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="416" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:6" ht="57.6">
       <c r="A416" s="2" t="s">
         <v>155</v>
       </c>
@@ -8995,7 +9333,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="417" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:6" ht="43.2">
       <c r="A417" s="2" t="s">
         <v>5</v>
       </c>
@@ -9015,7 +9353,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="418" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:6" ht="72">
       <c r="A418" s="2" t="s">
         <v>668</v>
       </c>
@@ -9035,7 +9373,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="419" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:6" ht="57.6">
       <c r="A419" s="2" t="s">
         <v>674</v>
       </c>
@@ -9055,7 +9393,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="420" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:6" ht="28.8">
       <c r="A420" s="2" t="s">
         <v>678</v>
       </c>
@@ -9075,7 +9413,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="421" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:6" ht="43.2">
       <c r="A421" s="2" t="s">
         <v>682</v>
       </c>
@@ -9095,7 +9433,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="422" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:6" ht="43.2">
       <c r="A422" s="2" t="s">
         <v>687</v>
       </c>
@@ -9115,7 +9453,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="423" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:6" ht="43.2">
       <c r="A423" s="2" t="s">
         <v>411</v>
       </c>
@@ -9135,7 +9473,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="424" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:6" ht="28.8">
       <c r="A424" s="2" t="s">
         <v>692</v>
       </c>
@@ -9155,7 +9493,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="425" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:6" ht="28.8">
       <c r="A425" s="2" t="s">
         <v>16</v>
       </c>
@@ -9175,17 +9513,17 @@
         <v>699</v>
       </c>
     </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A427" s="14" t="s">
+    <row r="427" spans="1:6">
+      <c r="A427" s="21" t="s">
         <v>739</v>
       </c>
-      <c r="B427" s="14"/>
-      <c r="C427" s="14"/>
-      <c r="D427" s="14"/>
-      <c r="E427" s="14"/>
-      <c r="F427" s="14"/>
-    </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B427" s="21"/>
+      <c r="C427" s="21"/>
+      <c r="D427" s="21"/>
+      <c r="E427" s="21"/>
+      <c r="F427" s="21"/>
+    </row>
+    <row r="428" spans="1:6">
       <c r="A428" s="1" t="s">
         <v>20</v>
       </c>
@@ -9205,7 +9543,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="429" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:6" ht="28.8">
       <c r="A429" s="2" t="s">
         <v>724</v>
       </c>
@@ -9223,7 +9561,7 @@
       </c>
       <c r="F429" s="2"/>
     </row>
-    <row r="430" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:6" ht="43.2">
       <c r="A430" s="2" t="s">
         <v>674</v>
       </c>
@@ -9243,7 +9581,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="431" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:6" ht="28.8">
       <c r="A431" s="2" t="s">
         <v>678</v>
       </c>
@@ -9263,7 +9601,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="432" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:6" ht="28.8">
       <c r="A432" s="2" t="s">
         <v>668</v>
       </c>
@@ -9283,7 +9621,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="433" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:6" ht="28.8">
       <c r="A433" s="2" t="s">
         <v>733</v>
       </c>
@@ -9301,7 +9639,7 @@
       </c>
       <c r="F433" s="2"/>
     </row>
-    <row r="434" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:6" ht="28.8">
       <c r="A434" s="2" t="s">
         <v>5</v>
       </c>
@@ -9319,7 +9657,7 @@
       </c>
       <c r="F434" s="2"/>
     </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:6">
       <c r="A435" s="2" t="s">
         <v>411</v>
       </c>
@@ -9337,7 +9675,7 @@
       </c>
       <c r="F435" s="2"/>
     </row>
-    <row r="436" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:6" ht="28.8">
       <c r="A436" s="2" t="s">
         <v>16</v>
       </c>
@@ -9357,25 +9695,21 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A209:F209"/>
-    <mergeCell ref="A339:F339"/>
-    <mergeCell ref="A341:F341"/>
-    <mergeCell ref="A352:F352"/>
-    <mergeCell ref="A361:F361"/>
-    <mergeCell ref="A321:E321"/>
-    <mergeCell ref="A329:E329"/>
-    <mergeCell ref="A281:E281"/>
-    <mergeCell ref="A297:E297"/>
-    <mergeCell ref="A150:F150"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A152:E152"/>
-    <mergeCell ref="A158:E158"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A119:F119"/>
-    <mergeCell ref="A100:F100"/>
-    <mergeCell ref="A90:F90"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A427:F427"/>
+    <mergeCell ref="A371:F371"/>
+    <mergeCell ref="A306:E306"/>
+    <mergeCell ref="A312:E312"/>
+    <mergeCell ref="A221:F221"/>
+    <mergeCell ref="A223:F223"/>
+    <mergeCell ref="A279:F279"/>
+    <mergeCell ref="A295:F295"/>
+    <mergeCell ref="A263:F263"/>
+    <mergeCell ref="A411:F411"/>
+    <mergeCell ref="A413:F413"/>
+    <mergeCell ref="A248:F248"/>
+    <mergeCell ref="A379:F379"/>
+    <mergeCell ref="A381:E381"/>
+    <mergeCell ref="A395:E395"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A237:E237"/>
     <mergeCell ref="A110:F110"/>
@@ -9392,21 +9726,25 @@
     <mergeCell ref="A190:F190"/>
     <mergeCell ref="A197:F197"/>
     <mergeCell ref="A138:F138"/>
-    <mergeCell ref="A427:F427"/>
-    <mergeCell ref="A371:F371"/>
-    <mergeCell ref="A306:E306"/>
-    <mergeCell ref="A312:E312"/>
-    <mergeCell ref="A221:F221"/>
-    <mergeCell ref="A223:F223"/>
-    <mergeCell ref="A279:F279"/>
-    <mergeCell ref="A295:F295"/>
-    <mergeCell ref="A263:F263"/>
-    <mergeCell ref="A411:F411"/>
-    <mergeCell ref="A413:F413"/>
-    <mergeCell ref="A248:F248"/>
-    <mergeCell ref="A379:F379"/>
-    <mergeCell ref="A381:E381"/>
-    <mergeCell ref="A395:E395"/>
+    <mergeCell ref="A150:F150"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A152:E152"/>
+    <mergeCell ref="A158:E158"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A119:F119"/>
+    <mergeCell ref="A100:F100"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="A80:F80"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A209:F209"/>
+    <mergeCell ref="A339:F339"/>
+    <mergeCell ref="A341:F341"/>
+    <mergeCell ref="A352:F352"/>
+    <mergeCell ref="A361:F361"/>
+    <mergeCell ref="A321:E321"/>
+    <mergeCell ref="A329:E329"/>
+    <mergeCell ref="A281:E281"/>
+    <mergeCell ref="A297:E297"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="32" orientation="portrait" horizontalDpi="300" r:id="rId1"/>

</xml_diff>